<commit_message>
Fixed description about the summer school
</commit_message>
<xml_diff>
--- a/springschooltable.xlsx
+++ b/springschooltable.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28518"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikiko\Dropbox\enPIT\20170811ESSロボチャレ\ESS2017RC-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nel/src/ESS2017RC/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18630" windowHeight="6570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20560" windowHeight="17800"/>
   </bookViews>
   <sheets>
     <sheet name="Program2017" sheetId="2" r:id="rId1"/>
     <sheet name="houkoku" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Program2017!$B$2:$F$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Program2017!$A$2:$G$33</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>日時</t>
     <rPh sb="0" eb="2">
@@ -418,6 +424,10 @@
     <rPh sb="15" eb="17">
       <t>ダイガク</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■2017サマースクール</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -425,7 +435,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,72 +502,72 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -567,7 +577,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -575,25 +585,25 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,159 +612,159 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -762,10 +772,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -773,10 +783,10 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -784,24 +794,24 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -809,34 +819,34 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,68 +855,68 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -917,25 +927,25 @@
         <color theme="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -982,7 +992,7 @@
         <color theme="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color theme="1"/>
@@ -994,10 +1004,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color theme="1"/>
@@ -1009,7 +1019,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color theme="1"/>
@@ -1072,156 +1082,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1232,6 +1092,90 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1244,20 +1188,86 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1542,377 +1552,377 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="B2" sqref="A2:G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.75" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.125" style="1"/>
+    <col min="5" max="5" width="28.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-    </row>
-    <row r="2" spans="1:7" ht="18.600000000000001" customHeight="1">
-      <c r="B2" s="81" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="83"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="79" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="80"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="21" t="s">
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B4" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="27" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="28"/>
-      <c r="C6" s="32" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="34"/>
+      <c r="C6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="73" t="s">
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="29.45" customHeight="1">
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42" t="s">
+      <c r="D10" s="52"/>
+      <c r="E10" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="42"/>
-    </row>
-    <row r="11" spans="1:7" s="6" customFormat="1">
-      <c r="B11" s="74" t="s">
+      <c r="F10" s="52"/>
+    </row>
+    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="76" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="78"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="45" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="47" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="38"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="F14" s="48"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="51"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="B17" s="21" t="s">
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B17" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="21" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B18" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="21" t="s">
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B19" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="70"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="B21" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="B22" s="21" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B21" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B22" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B25" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B26" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B27" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B28" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="B29" s="21" t="s">
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B29" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="23"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="28"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B30" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B31" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B32" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -1969,245 +1979,245 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="1"/>
-    <col min="2" max="2" width="11.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.125" style="1"/>
+    <col min="5" max="5" width="28.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15" thickBot="1">
+    <row r="1" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="43" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="45"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="46" t="s">
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B3" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="47"/>
-      <c r="C4" s="32" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="62"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B4" s="61"/>
+      <c r="C4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="49"/>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="63"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="50"/>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="64"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="51"/>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="65"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="51"/>
-    </row>
-    <row r="8" spans="2:6" s="6" customFormat="1" ht="29.45" customHeight="1">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="65"/>
+    </row>
+    <row r="8" spans="2:6" s="6" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="52"/>
-    </row>
-    <row r="9" spans="2:6" s="6" customFormat="1" ht="15" thickBot="1">
+      <c r="F8" s="66"/>
+    </row>
+    <row r="9" spans="2:6" s="6" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="54"/>
-    </row>
-    <row r="10" spans="2:6" ht="15" thickBot="1"/>
-    <row r="11" spans="2:6" ht="15" thickBot="1">
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="68"/>
+    </row>
+    <row r="10" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="43" t="s">
+      <c r="D11" s="58"/>
+      <c r="E11" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="45"/>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="F11" s="59"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="71" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="72" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="59"/>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="F13" s="73"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="60"/>
-    </row>
-    <row r="15" spans="2:6" ht="15" thickBot="1">
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="74"/>
+    </row>
+    <row r="15" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="63"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1"/>
-    <row r="17" spans="2:6" ht="15" thickBot="1">
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="77"/>
+    </row>
+    <row r="16" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="43" t="s">
+      <c r="D17" s="58"/>
+      <c r="E17" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="45"/>
-    </row>
-    <row r="18" spans="2:6" ht="30" customHeight="1">
+      <c r="F17" s="59"/>
+    </row>
+    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="65"/>
-    </row>
-    <row r="19" spans="2:6" ht="28.5" customHeight="1" thickBot="1">
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="79"/>
+    </row>
+    <row r="19" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
-    </row>
-    <row r="20" spans="2:6" ht="15" thickBot="1"/>
-    <row r="21" spans="2:6" ht="15" thickBot="1">
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="81"/>
+    </row>
+    <row r="20" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="43" t="s">
+      <c r="D21" s="58"/>
+      <c r="E21" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="45"/>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="F21" s="59"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
-    </row>
-    <row r="23" spans="2:6" ht="15" thickBot="1">
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="83"/>
+    </row>
+    <row r="23" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="56"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>